<commit_message>
cleaning up analysis for MS
</commit_message>
<xml_diff>
--- a/04_RESULTS/COMP1_results_summary.xlsx
+++ b/04_RESULTS/COMP1_results_summary.xlsx
@@ -8,20 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelsmith/Documents/00_UQ_offline/STJW_analysis/04_RESULTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E85B98-BFDF-F747-960C-717A344141CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651A2E12-8DF7-914E-9F05-0F3D92EE6E32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIVERSITY_RESULTS_SUMMARY" sheetId="1" r:id="rId1"/>
     <sheet name="INVIV_SPECIES_SUMMARY" sheetId="2" r:id="rId2"/>
+    <sheet name="Table_S1_func_group_summary" sheetId="3" r:id="rId3"/>
+    <sheet name="Table_S2_reserve_effects" sheetId="4" r:id="rId4"/>
+    <sheet name="Table_S3_individual_species" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="166">
   <si>
     <t>group</t>
   </si>
@@ -389,9 +403,6 @@
     <t>fit_abund</t>
   </si>
   <si>
-    <t>abund</t>
-  </si>
-  <si>
     <t>binom_2wayP</t>
   </si>
   <si>
@@ -438,14 +449,99 @@
   </si>
   <si>
     <t>*predictions not reliable; model not fitting</t>
+  </si>
+  <si>
+    <t>Functional Group</t>
+  </si>
+  <si>
+    <t>No. observations</t>
+  </si>
+  <si>
+    <t>Proportion zeros</t>
+  </si>
+  <si>
+    <t>Models fitted</t>
+  </si>
+  <si>
+    <t>Binomial</t>
+  </si>
+  <si>
+    <t>Richness &amp; diversity</t>
+  </si>
+  <si>
+    <t>Three-way</t>
+  </si>
+  <si>
+    <t>Two-way</t>
+  </si>
+  <si>
+    <t>Richness</t>
+  </si>
+  <si>
+    <t>Diversity</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Lifespan</t>
+  </si>
+  <si>
+    <t>Functional group</t>
+  </si>
+  <si>
+    <t>Proportion zero</t>
+  </si>
+  <si>
+    <t>Abundance</t>
+  </si>
+  <si>
+    <t>Forb</t>
+  </si>
+  <si>
+    <t>Leguminous forb</t>
+  </si>
+  <si>
+    <t>Two-way P</t>
+  </si>
+  <si>
+    <t>Three-way P</t>
+  </si>
+  <si>
+    <t>Total count</t>
+  </si>
+  <si>
+    <t>abund**</t>
+  </si>
+  <si>
+    <t>** this 'abund' column is actually</t>
+  </si>
+  <si>
+    <t>the number of plots with abundance data</t>
+  </si>
+  <si>
+    <t>this value is the inverse of the 'proportion zeros' column</t>
+  </si>
+  <si>
+    <t>When expressed as a proportion of the total number of plots (144)</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -992,7 +1088,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1042,6 +1138,10 @@
     <xf numFmtId="164" fontId="20" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,10 +1157,54 @@
     <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="18" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1419,12 +1563,12 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
@@ -1446,32 +1590,32 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="28"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31" t="s">
+      <c r="K1" s="32"/>
+      <c r="L1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="27" t="s">
+      <c r="M1" s="33"/>
+      <c r="N1" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3198,10 +3342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A407081-6980-F948-92B6-61488ECCD3D9}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3230,28 +3374,28 @@
   <sheetData>
     <row r="1" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>121</v>
@@ -3266,31 +3410,31 @@
         <v>118</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P1" s="18" t="s">
         <v>85</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T1" s="18" t="s">
         <v>29</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.15">
@@ -3457,8 +3601,8 @@
       <c r="K4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>137</v>
+      <c r="L4" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>86</v>
@@ -4203,10 +4347,2167 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.15">
-      <c r="L17" s="33" t="s">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.15">
+      <c r="H17" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.15">
+      <c r="H18" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.15">
+      <c r="H19" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.15">
+      <c r="H20" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8EE5B0-7C38-844D-83D3-DA62D896875B}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="38"/>
+      <c r="F1" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3073</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0.73480000000000001</v>
+      </c>
+      <c r="I3" s="40">
+        <v>0.37490000000000001</v>
+      </c>
+      <c r="J3" s="41">
+        <v>0.30180000000000001</v>
+      </c>
+      <c r="K3" s="41">
+        <v>0.2283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2305</v>
+      </c>
+      <c r="C4" s="37">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="40">
+        <v>0.51910000000000001</v>
+      </c>
+      <c r="I4" s="40">
+        <v>0.84450000000000003</v>
+      </c>
+      <c r="J4" s="41">
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="K4" s="41">
+        <v>0.17749999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1">
+        <v>768</v>
+      </c>
+      <c r="C5" s="37">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="40">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="I5" s="44">
+        <v>0</v>
+      </c>
+      <c r="J5" s="41">
+        <v>0.22420000000000001</v>
+      </c>
+      <c r="K5" s="41">
+        <v>0.33389999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1195</v>
+      </c>
+      <c r="C6" s="37">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="40">
+        <v>0.56740000000000002</v>
+      </c>
+      <c r="I6" s="40">
+        <v>0.75049999999999994</v>
+      </c>
+      <c r="J6" s="41">
+        <v>0.63429999999999997</v>
+      </c>
+      <c r="K6" s="41">
+        <v>0.13469999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1">
+        <v>823</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0.6754</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="J7" s="41">
+        <v>0.55959999999999999</v>
+      </c>
+      <c r="K7" s="41">
+        <v>0.59570000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1">
+        <v>372</v>
+      </c>
+      <c r="C8" s="37">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0.4617</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="J8" s="45">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1110</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="40">
+        <v>0.78190000000000004</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0.83030000000000004</v>
+      </c>
+      <c r="J9" s="41">
+        <v>0.48110000000000003</v>
+      </c>
+      <c r="K9" s="41">
+        <v>0.14940000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1">
+        <v>236</v>
+      </c>
+      <c r="C10" s="37">
+        <v>0.15972222222222221</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="40">
+        <v>0.28860000000000002</v>
+      </c>
+      <c r="I10" s="40">
+        <v>0.24590000000000001</v>
+      </c>
+      <c r="J10" s="41">
+        <v>0.2203</v>
+      </c>
+      <c r="K10" s="41">
+        <v>0.84540000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1">
+        <v>532</v>
+      </c>
+      <c r="C11" s="37">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="39">
+        <v>0.59668470406251595</v>
+      </c>
+      <c r="G11" s="39">
+        <v>0.54251543269230296</v>
+      </c>
+      <c r="H11" s="40">
+        <v>0.25319999999999998</v>
+      </c>
+      <c r="I11" s="40">
+        <v>1</v>
+      </c>
+      <c r="J11" s="41">
+        <v>0.1157</v>
+      </c>
+      <c r="K11" s="41">
+        <v>0.44490000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1298</v>
+      </c>
+      <c r="C12" s="37">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="40">
+        <v>0.68269999999999997</v>
+      </c>
+      <c r="I12" s="40">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="J12" s="41">
+        <v>0.72629999999999995</v>
+      </c>
+      <c r="K12" s="41">
+        <v>5.5399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1">
+        <v>537</v>
+      </c>
+      <c r="C13" s="37">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="40">
+        <v>0.1595</v>
+      </c>
+      <c r="I13" s="44">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J13" s="41">
+        <v>0.1303</v>
+      </c>
+      <c r="K13" s="41">
+        <v>8.3099999999999993E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1">
+        <v>424</v>
+      </c>
+      <c r="C14" s="37">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="39">
+        <v>0.67936157811425002</v>
+      </c>
+      <c r="G14" s="39">
+        <v>0.14798711145694601</v>
+      </c>
+      <c r="H14" s="44">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="I14" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="45">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1">
+        <v>113</v>
+      </c>
+      <c r="C15" s="37">
+        <v>0.3125</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="39">
+        <v>0.76242480909532895</v>
+      </c>
+      <c r="G15" s="39">
+        <v>0.34011786664647697</v>
+      </c>
+      <c r="H15" s="40">
+        <v>1</v>
+      </c>
+      <c r="I15" s="40">
+        <v>1</v>
+      </c>
+      <c r="J15" s="41">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="K15" s="41">
+        <v>0.77549999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1">
+        <v>215</v>
+      </c>
+      <c r="C16" s="37">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="40">
+        <v>0.92459999999999998</v>
+      </c>
+      <c r="I16" s="40">
+        <v>0.96179999999999999</v>
+      </c>
+      <c r="J16" s="41">
+        <v>0.45619999999999999</v>
+      </c>
+      <c r="K16" s="41">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1083</v>
+      </c>
+      <c r="C17" s="37">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="40">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="I17" s="40">
+        <v>0.57640000000000002</v>
+      </c>
+      <c r="J17" s="41">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="K17" s="41">
+        <v>0.46579999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1170</v>
+      </c>
+      <c r="C18" s="37">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="40">
+        <v>0.81140000000000001</v>
+      </c>
+      <c r="I18" s="40">
+        <v>0.92310000000000003</v>
+      </c>
+      <c r="J18" s="41">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="K18" s="41">
+        <v>0.2407</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1">
+        <v>329</v>
+      </c>
+      <c r="C19" s="37">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="40">
+        <v>0.21590000000000001</v>
+      </c>
+      <c r="I19" s="40">
+        <v>0.47810000000000002</v>
+      </c>
+      <c r="J19" s="41">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="K19" s="41">
+        <v>0.60770000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1">
+        <v>128</v>
+      </c>
+      <c r="C20" s="37">
+        <v>0.375</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="46">
+        <v>3.0865651583756901E-2</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="40">
+        <v>1</v>
+      </c>
+      <c r="I20" s="40">
+        <v>1</v>
+      </c>
+      <c r="J20" s="41">
+        <v>0.2087</v>
+      </c>
+      <c r="K20" s="41">
+        <v>0.32050000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1">
+        <v>208</v>
+      </c>
+      <c r="C21" s="37">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="39">
+        <v>0.216686556711852</v>
+      </c>
+      <c r="G21" s="46">
+        <v>2.8493285089524201E-3</v>
+      </c>
+      <c r="H21" s="40">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="I21" s="40">
+        <v>1</v>
+      </c>
+      <c r="J21" s="41">
+        <v>0.29870000000000002</v>
+      </c>
+      <c r="K21" s="45">
+        <v>3.73E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1">
+        <v>955</v>
+      </c>
+      <c r="C22" s="37">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="40">
+        <v>0.72819999999999996</v>
+      </c>
+      <c r="I22" s="40">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="J22" s="41">
+        <v>0.48259999999999997</v>
+      </c>
+      <c r="K22" s="41">
+        <v>0.1905</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1">
+        <v>231</v>
+      </c>
+      <c r="C23" s="37">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="39">
+        <v>0.41076893214743498</v>
+      </c>
+      <c r="G23" s="39">
+        <v>0.91159942440487396</v>
+      </c>
+      <c r="H23" s="40">
+        <v>1</v>
+      </c>
+      <c r="I23" s="40">
+        <v>1</v>
+      </c>
+      <c r="J23" s="41">
+        <v>0.77949999999999997</v>
+      </c>
+      <c r="K23" s="41">
+        <v>0.20680000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1">
+        <v>226</v>
+      </c>
+      <c r="C24" s="37">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="39">
+        <v>0.41076893214743498</v>
+      </c>
+      <c r="G24" s="39">
+        <v>0.91159942440487396</v>
+      </c>
+      <c r="H24" s="40">
+        <v>1</v>
+      </c>
+      <c r="I24" s="40">
+        <v>1</v>
+      </c>
+      <c r="J24" s="41">
+        <v>0.69510000000000005</v>
+      </c>
+      <c r="K24" s="41">
+        <v>0.22450000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="1">
+        <v>5</v>
+      </c>
+      <c r="C25" s="37">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="39">
+        <v>0.85182104561004501</v>
+      </c>
+      <c r="G25" s="39">
+        <v>0.94588042864084099</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1">
+        <v>823</v>
+      </c>
+      <c r="C26" s="37">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="40">
+        <v>0.98580000000000001</v>
+      </c>
+      <c r="I26" s="40">
+        <v>0.57410000000000005</v>
+      </c>
+      <c r="J26" s="41">
+        <v>0.45679999999999998</v>
+      </c>
+      <c r="K26" s="41">
+        <v>8.1699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="1">
+        <v>595</v>
+      </c>
+      <c r="C27" s="37">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="40">
+        <v>0.97230000000000005</v>
+      </c>
+      <c r="I27" s="40">
+        <v>0.97240000000000004</v>
+      </c>
+      <c r="J27" s="41">
+        <v>0.35439999999999999</v>
+      </c>
+      <c r="K27" s="41">
+        <v>9.1300000000000006E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="1">
+        <v>360</v>
+      </c>
+      <c r="C28" s="37">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="40">
+        <v>0.37259999999999999</v>
+      </c>
+      <c r="I28" s="40">
+        <v>0.87370000000000003</v>
+      </c>
+      <c r="J28" s="41">
+        <v>0.4007</v>
+      </c>
+      <c r="K28" s="41">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="1">
+        <v>228</v>
+      </c>
+      <c r="C29" s="37">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="39">
+        <v>0.41076893214743498</v>
+      </c>
+      <c r="G29" s="39">
+        <v>0.91159942440487396</v>
+      </c>
+      <c r="H29" s="40">
+        <v>1</v>
+      </c>
+      <c r="I29" s="40">
+        <v>1</v>
+      </c>
+      <c r="J29" s="41">
+        <v>0.8115</v>
+      </c>
+      <c r="K29" s="41">
+        <v>0.19320000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1">
+        <v>27</v>
+      </c>
+      <c r="C30" s="37">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="39">
+        <v>8.0904505081459105E-2</v>
+      </c>
+      <c r="G30" s="39">
+        <v>0.114372414340387</v>
+      </c>
+      <c r="H30" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436F4BEA-6809-4940-8020-84F45D5A92F0}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="43">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="E3" s="43">
+        <v>0</v>
+      </c>
+      <c r="F3" s="43">
+        <v>0.2114</v>
+      </c>
+      <c r="G3" s="43">
+        <v>8.8000000000000005E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="43">
+        <v>0.14810000000000001</v>
+      </c>
+      <c r="E4" s="43">
+        <v>1.49E-2</v>
+      </c>
+      <c r="F4" s="42">
+        <v>0.18290000000000001</v>
+      </c>
+      <c r="G4" s="42">
+        <v>7.2599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="43">
+        <v>0.47910000000000003</v>
+      </c>
+      <c r="E5" s="43">
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="42">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="G5" s="42">
+        <v>5.62E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="43">
+        <v>0.31940000000000002</v>
+      </c>
+      <c r="E6" s="43">
+        <v>0</v>
+      </c>
+      <c r="F6" s="43">
+        <v>0.2442</v>
+      </c>
+      <c r="G6" s="43">
+        <v>1.37E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="43">
+        <v>0.27139999999999997</v>
+      </c>
+      <c r="E7" s="43">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F7" s="43">
+        <v>0.24790000000000001</v>
+      </c>
+      <c r="G7" s="43">
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="43">
+        <v>0.42570000000000002</v>
+      </c>
+      <c r="E8" s="43">
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="42">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="E9" s="42">
+        <v>0.60750000000000004</v>
+      </c>
+      <c r="F9" s="42">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="G9" s="42">
+        <v>0.9365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="43">
+        <v>0.53639999999999999</v>
+      </c>
+      <c r="E10" s="43">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F10" s="42">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="G10" s="42">
+        <v>6.8199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="42">
+        <v>0.82989999999999997</v>
+      </c>
+      <c r="C11" s="42">
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="D11" s="43">
+        <v>0.45710000000000001</v>
+      </c>
+      <c r="E11" s="43">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F11" s="42">
+        <v>0.13039999999999999</v>
+      </c>
+      <c r="G11" s="42">
+        <v>0.29770000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="43">
+        <v>0.2833</v>
+      </c>
+      <c r="E12" s="43">
+        <v>1E-4</v>
+      </c>
+      <c r="F12" s="43">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="G12" s="43">
+        <v>3.0300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="43">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="E13" s="43">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F13" s="43">
+        <v>0.1777</v>
+      </c>
+      <c r="G13" s="43">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="43">
+        <v>2.0314000000000001</v>
+      </c>
+      <c r="C14" s="43">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="42">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="C15" s="42">
+        <v>0.19189999999999999</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0.1598</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0.39779999999999999</v>
+      </c>
+      <c r="F15" s="42">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="G15" s="42">
+        <v>0.57530000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="42">
+        <v>-7.1499999999999994E-2</v>
+      </c>
+      <c r="E16" s="42">
+        <v>0.65780000000000005</v>
+      </c>
+      <c r="F16" s="42">
+        <v>-3.56E-2</v>
+      </c>
+      <c r="G16" s="42">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="43">
+        <v>0.3538</v>
+      </c>
+      <c r="E17" s="43">
+        <v>0</v>
+      </c>
+      <c r="F17" s="43">
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="G17" s="43">
+        <v>1.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="43">
+        <v>0.30009999999999998</v>
+      </c>
+      <c r="E18" s="43">
+        <v>0</v>
+      </c>
+      <c r="F18" s="43">
+        <v>0.24310000000000001</v>
+      </c>
+      <c r="G18" s="43">
+        <v>1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="42">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="E19" s="42">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F19" s="42">
+        <v>-0.114</v>
+      </c>
+      <c r="G19" s="42">
+        <v>0.1303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="42">
+        <v>1.5531999999999999</v>
+      </c>
+      <c r="C20" s="42">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="D20" s="42">
+        <v>0.12529999999999999</v>
+      </c>
+      <c r="E20" s="42">
+        <v>0.48010000000000003</v>
+      </c>
+      <c r="F20" s="42">
+        <v>1.8E-3</v>
+      </c>
+      <c r="G20" s="42">
+        <v>0.98380000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="42">
+        <v>0.82989999999999997</v>
+      </c>
+      <c r="C21" s="42">
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="D21" s="43">
+        <v>1.3552999999999999</v>
+      </c>
+      <c r="E21" s="43">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F21" s="42">
+        <v>0.25359999999999999</v>
+      </c>
+      <c r="G21" s="42">
+        <v>7.0300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="42">
+        <v>-6.3100000000000003E-2</v>
+      </c>
+      <c r="E22" s="42">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="F22" s="42">
+        <v>3.44E-2</v>
+      </c>
+      <c r="G22" s="42">
+        <v>0.72060000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="42">
+        <v>1.2888999999999999</v>
+      </c>
+      <c r="C23" s="42">
+        <v>6.1400000000000003E-2</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="E23" s="43">
+        <v>1E-4</v>
+      </c>
+      <c r="F23" s="43">
+        <v>0.29360000000000003</v>
+      </c>
+      <c r="G23" s="43">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="43">
+        <v>2.0314000000000001</v>
+      </c>
+      <c r="C24" s="43">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="D24" s="43">
+        <v>0.5252</v>
+      </c>
+      <c r="E24" s="43">
+        <v>1E-4</v>
+      </c>
+      <c r="F24" s="43">
+        <v>0.28539999999999999</v>
+      </c>
+      <c r="G24" s="43">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="42">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="C25" s="42">
+        <v>0.19189999999999999</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="42">
+        <v>5.04E-2</v>
+      </c>
+      <c r="E26" s="42">
+        <v>0.54059999999999997</v>
+      </c>
+      <c r="F26" s="42">
+        <v>5.2900000000000003E-2</v>
+      </c>
+      <c r="G26" s="42">
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="42">
+        <v>-0.24299999999999999</v>
+      </c>
+      <c r="E27" s="42">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="F27" s="43">
+        <v>-0.2266</v>
+      </c>
+      <c r="G27" s="43">
+        <v>8.3999999999999995E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="43">
+        <v>0.52039999999999997</v>
+      </c>
+      <c r="E28" s="43">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F28" s="43">
+        <v>0.27650000000000002</v>
+      </c>
+      <c r="G28" s="43">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="42">
+        <v>0.82989999999999997</v>
+      </c>
+      <c r="C29" s="42">
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="D29" s="43">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="E29" s="43">
+        <v>0</v>
+      </c>
+      <c r="F29" s="43">
+        <v>0.2114</v>
+      </c>
+      <c r="G29" s="43">
+        <v>8.8000000000000005E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="42">
+        <v>1.5531999999999999</v>
+      </c>
+      <c r="C30" s="42">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5849B4CE-2A93-8A4C-9239-14AB27A29202}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="27" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="17" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="F1" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="49">
+        <v>1836</v>
+      </c>
+      <c r="E3" s="51">
+        <v>0.104166667</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="52">
+        <v>0.97719999999999996</v>
+      </c>
+      <c r="I3" s="52">
+        <v>1</v>
+      </c>
+      <c r="J3" s="53">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="K3" s="52">
+        <v>0.1231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="49">
+        <v>369</v>
+      </c>
+      <c r="E4" s="51">
+        <v>0.51388888899999996</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="52">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="I4" s="53">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="49">
+        <v>1816</v>
+      </c>
+      <c r="E5" s="51">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="52">
+        <v>0.7429</v>
+      </c>
+      <c r="I5" s="52">
+        <v>1</v>
+      </c>
+      <c r="J5" s="53">
+        <v>0</v>
+      </c>
+      <c r="K5" s="52">
+        <v>0.69210000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="17">
+        <v>171</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.63888888899999996</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="47">
+        <v>0.1779</v>
+      </c>
+      <c r="I6" s="47">
+        <v>0.1125</v>
+      </c>
+      <c r="J6" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="17">
+        <v>260</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0.46527777799999998</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="47">
+        <v>0.32429999999999998</v>
+      </c>
+      <c r="I7" s="47">
+        <v>0.38419999999999999</v>
+      </c>
+      <c r="J7" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="K7" s="47">
+        <v>0.87280000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="17">
+        <v>847</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0.84722222199999997</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="47">
+        <v>1</v>
+      </c>
+      <c r="I8" s="47">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="J8" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="17">
+        <v>549</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0.34027777799999998</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="47">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="I9" s="47">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="J9" s="47">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="K9" s="47">
+        <v>0.63249999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="17">
+        <v>564</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0.70138888899999996</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="47">
+        <v>0.84489999999999998</v>
+      </c>
+      <c r="I10" s="47">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="J10" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J12" s="49"/>
+      <c r="K12" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating following bug fix
</commit_message>
<xml_diff>
--- a/04_RESULTS/COMP1_results_summary.xlsx
+++ b/04_RESULTS/COMP1_results_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelsmith/Documents/00_UQ_offline/STJW_analysis/04_RESULTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAA8D10-BCEC-8845-AEE5-B2763C6FAEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC34FF6-4098-0544-B659-41D2653CC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIVERSITY_RESULTS_SUMMARY" sheetId="1" r:id="rId1"/>
@@ -1334,6 +1334,13 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1351,13 +1358,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1744,32 +1744,32 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="47"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="49" t="s">
+      <c r="I1" s="51"/>
+      <c r="J1" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="50"/>
-      <c r="N1" s="46" t="s">
+      <c r="M1" s="53"/>
+      <c r="N1" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -4533,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8EE5B0-7C38-844D-83D3-DA62D896875B}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4556,22 +4556,22 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49" t="s">
+      <c r="G1" s="51"/>
+      <c r="H1" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="50"/>
+      <c r="K1" s="53"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -5603,7 +5603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D6818A-1E2A-3A40-B8DF-9DF8925E0E91}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -5621,20 +5621,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46" t="s">
+      <c r="E1" s="49"/>
+      <c r="F1" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="46"/>
-    </row>
-    <row r="2" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="49"/>
+    </row>
+    <row r="2" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>138</v>
       </c>
@@ -5662,22 +5662,22 @@
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="54" t="s">
+      <c r="B3" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="48">
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
@@ -5685,22 +5685,22 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="54" t="s">
+      <c r="B4" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="48">
         <v>1.49E-2</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="46">
         <v>7.2599999999999998E-2</v>
       </c>
     </row>
@@ -5708,22 +5708,22 @@
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="54" t="s">
+      <c r="B5" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="46">
         <v>5.62E-2</v>
       </c>
     </row>
@@ -5731,22 +5731,22 @@
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="54" t="s">
+      <c r="B6" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="48">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="48">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
@@ -5754,22 +5754,22 @@
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="54" t="s">
+      <c r="B7" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F7" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="52" t="s">
+      <c r="F7" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="46" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5777,22 +5777,22 @@
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="54" t="s">
+      <c r="B8" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="48">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="46">
         <v>6.8199999999999997E-2</v>
       </c>
     </row>
@@ -5800,22 +5800,22 @@
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="46">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="48">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="46">
         <v>0.29770000000000002</v>
       </c>
     </row>
@@ -5823,22 +5823,22 @@
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="52" t="s">
+      <c r="B10" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="46">
         <v>0.60750000000000004</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="46">
         <v>0.9365</v>
       </c>
     </row>
@@ -5846,22 +5846,22 @@
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="54" t="s">
+      <c r="B11" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F11" s="54" t="s">
+      <c r="F11" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="48">
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
@@ -5869,22 +5869,22 @@
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="54" t="s">
+      <c r="B12" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="48">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F12" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="54">
+      <c r="G12" s="48">
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
@@ -5892,22 +5892,22 @@
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="48">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="52" t="s">
+      <c r="D13" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="46" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5915,22 +5915,22 @@
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="C14" s="52">
+      <c r="C14" s="46">
         <v>0.19189999999999999</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="46">
         <v>0.39779999999999999</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="46" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="46">
         <v>0.57530000000000003</v>
       </c>
     </row>
@@ -5938,22 +5938,22 @@
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="52" t="s">
+      <c r="B15" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="46">
         <v>0.65780000000000005</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="G15" s="52">
+      <c r="G15" s="46">
         <v>0.59699999999999998</v>
       </c>
     </row>
@@ -5961,22 +5961,22 @@
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="54" t="s">
+      <c r="B16" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="G16" s="54">
+      <c r="G16" s="48">
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
@@ -5984,22 +5984,22 @@
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="54" t="s">
+      <c r="B17" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="48">
         <v>1.1299999999999999E-2</v>
       </c>
     </row>
@@ -6007,22 +6007,22 @@
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="52" t="s">
+      <c r="B18" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="46">
         <v>0.69599999999999995</v>
       </c>
-      <c r="F18" s="52" t="s">
+      <c r="F18" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G18" s="46">
         <v>0.1303</v>
       </c>
     </row>
@@ -6030,22 +6030,22 @@
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C19" s="46">
         <v>0.24629999999999999</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="46">
         <v>0.48010000000000003</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G19" s="46">
         <v>0.98380000000000001</v>
       </c>
     </row>
@@ -6053,22 +6053,22 @@
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="C20" s="52">
+      <c r="C20" s="46">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F20" s="52" t="s">
+      <c r="F20" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="46">
         <v>7.0300000000000001E-2</v>
       </c>
     </row>
@@ -6076,22 +6076,22 @@
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="52" t="s">
+      <c r="B21" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="46">
         <v>0.42270000000000002</v>
       </c>
-      <c r="F21" s="52" t="s">
+      <c r="F21" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="G21" s="52">
+      <c r="G21" s="46">
         <v>0.72060000000000002</v>
       </c>
     </row>
@@ -6099,22 +6099,22 @@
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="52">
+      <c r="C22" s="46">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="E22" s="54" t="s">
+      <c r="E22" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="G22" s="54" t="s">
+      <c r="G22" s="48" t="s">
         <v>216</v>
       </c>
     </row>
@@ -6122,22 +6122,22 @@
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="48">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="G23" s="54" t="s">
+      <c r="G23" s="48" t="s">
         <v>216</v>
       </c>
     </row>
@@ -6145,22 +6145,22 @@
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="C24" s="52">
+      <c r="C24" s="46">
         <v>0.19189999999999999</v>
       </c>
-      <c r="D24" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="52" t="s">
+      <c r="D24" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="46" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6168,22 +6168,22 @@
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="52" t="s">
+      <c r="B25" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="46">
         <v>0.54059999999999997</v>
       </c>
-      <c r="F25" s="52" t="s">
+      <c r="F25" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="46">
         <v>0.51200000000000001</v>
       </c>
     </row>
@@ -6191,22 +6191,22 @@
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="52" t="s">
+      <c r="B26" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="46">
         <v>9.8599999999999993E-2</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G26" s="48">
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
@@ -6214,22 +6214,22 @@
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="54" t="s">
+      <c r="B27" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F27" s="54" t="s">
+      <c r="F27" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="54">
+      <c r="G27" s="48">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
@@ -6237,22 +6237,22 @@
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="C28" s="52">
+      <c r="C28" s="46">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="54" t="s">
+      <c r="F28" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="G28" s="54">
+      <c r="G28" s="48">
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
@@ -6260,22 +6260,22 @@
       <c r="A29" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="C29" s="52">
+      <c r="C29" s="46">
         <v>0.24629999999999999</v>
       </c>
-      <c r="D29" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="52" t="s">
+      <c r="D29" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="46" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor summaries for paper
</commit_message>
<xml_diff>
--- a/04_RESULTS/COMP1_results_summary.xlsx
+++ b/04_RESULTS/COMP1_results_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelsmith/Documents/00_UQ_offline/STJW_analysis/04_RESULTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC34FF6-4098-0544-B659-41D2653CC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96843638-009C-5A44-A8EB-924961E8FA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIVERSITY_RESULTS_SUMMARY" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="218">
   <si>
     <t>group</t>
   </si>
@@ -686,6 +686,9 @@
   </si>
   <si>
     <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>No. species</t>
   </si>
 </sst>
 </file>
@@ -1295,11 +1298,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="18" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1341,6 +1340,9 @@
     <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1359,6 +1361,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1744,32 +1747,32 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="50"/>
+      <c r="J1" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="53"/>
-      <c r="N1" s="49" t="s">
+      <c r="M1" s="52"/>
+      <c r="N1" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -4531,1069 +4534,1158 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8EE5B0-7C38-844D-83D3-DA62D896875B}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="54" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="53"/>
+      <c r="G1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="51"/>
+      <c r="K1" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="53"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="52"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1">
+        <v>119</v>
+      </c>
+      <c r="C3" s="1">
         <v>3073</v>
       </c>
-      <c r="C3" s="32">
+      <c r="D3" s="30">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="34">
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="32">
         <v>0.73480000000000001</v>
       </c>
-      <c r="I3" s="34">
+      <c r="J3" s="32">
         <v>0.37490000000000001</v>
       </c>
-      <c r="J3" s="35">
+      <c r="K3" s="33">
         <v>0.30180000000000001</v>
       </c>
-      <c r="K3" s="35">
+      <c r="L3" s="33">
         <v>0.2283</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1">
         <v>2305</v>
       </c>
-      <c r="C4" s="32">
+      <c r="D4" s="30">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="34">
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="32">
         <v>0.51910000000000001</v>
       </c>
-      <c r="I4" s="34">
+      <c r="J4" s="32">
         <v>0.84450000000000003</v>
       </c>
-      <c r="J4" s="35">
+      <c r="K4" s="33">
         <v>0.62280000000000002</v>
       </c>
-      <c r="K4" s="35">
+      <c r="L4" s="33">
         <v>0.17749999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="1">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1">
         <v>768</v>
       </c>
-      <c r="C5" s="32">
+      <c r="D5" s="30">
         <v>7.6388888888888895E-2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="34">
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="32">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="I5" s="36">
+      <c r="J5" s="34">
         <v>0</v>
       </c>
-      <c r="J5" s="35">
+      <c r="K5" s="33">
         <v>0.22420000000000001</v>
       </c>
-      <c r="K5" s="35">
+      <c r="L5" s="33">
         <v>0.33389999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="1">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1">
         <v>1195</v>
       </c>
-      <c r="C6" s="32">
+      <c r="D6" s="30">
         <v>0</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="34">
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="32">
         <v>0.56740000000000002</v>
       </c>
-      <c r="I6" s="34">
+      <c r="J6" s="32">
         <v>0.75049999999999994</v>
       </c>
-      <c r="J6" s="35">
+      <c r="K6" s="33">
         <v>0.63429999999999997</v>
       </c>
-      <c r="K6" s="35">
+      <c r="L6" s="33">
         <v>0.13469999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="1">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1">
         <v>823</v>
       </c>
-      <c r="C7" s="32">
+      <c r="D7" s="30">
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="34">
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="32">
         <v>0.6754</v>
       </c>
-      <c r="I7" s="34">
+      <c r="J7" s="32">
         <v>0.67100000000000004</v>
       </c>
-      <c r="J7" s="35">
+      <c r="K7" s="33">
         <v>0.55959999999999999</v>
       </c>
-      <c r="K7" s="35">
+      <c r="L7" s="33">
         <v>0.59570000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
         <v>372</v>
       </c>
-      <c r="C8" s="32">
+      <c r="D8" s="30">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="34">
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="32">
         <v>0.4617</v>
       </c>
-      <c r="I8" s="34">
+      <c r="J8" s="32">
         <v>0.98409999999999997</v>
       </c>
-      <c r="J8" s="37">
+      <c r="K8" s="35">
         <v>1.8E-3</v>
       </c>
-      <c r="K8" s="35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>236</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.15972222222222221</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0.28860000000000002</v>
+      </c>
+      <c r="J9" s="32">
+        <v>0.24590000000000001</v>
+      </c>
+      <c r="K9" s="33">
+        <v>0.2203</v>
+      </c>
+      <c r="L9" s="33">
+        <v>0.84540000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1">
+        <v>532</v>
+      </c>
+      <c r="D10" s="30">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="31">
+        <v>0.59668470406251595</v>
+      </c>
+      <c r="H10" s="31">
+        <v>0.54251543269230296</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0.25319999999999998</v>
+      </c>
+      <c r="J10" s="32">
+        <v>1</v>
+      </c>
+      <c r="K10" s="33">
+        <v>0.1157</v>
+      </c>
+      <c r="L10" s="33">
+        <v>0.44490000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B11" s="1">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1">
         <v>1110</v>
       </c>
-      <c r="C9" s="32">
+      <c r="D11" s="30">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="34">
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="32">
         <v>0.78190000000000004</v>
       </c>
-      <c r="I9" s="34">
+      <c r="J11" s="32">
         <v>0.83030000000000004</v>
       </c>
-      <c r="J9" s="35">
+      <c r="K11" s="33">
         <v>0.48110000000000003</v>
       </c>
-      <c r="K9" s="35">
+      <c r="L11" s="33">
         <v>0.14940000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1">
-        <v>236</v>
-      </c>
-      <c r="C10" s="32">
-        <v>0.15972222222222221</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="34">
-        <v>0.28860000000000002</v>
-      </c>
-      <c r="I10" s="34">
-        <v>0.24590000000000001</v>
-      </c>
-      <c r="J10" s="35">
-        <v>0.2203</v>
-      </c>
-      <c r="K10" s="35">
-        <v>0.84540000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="1">
-        <v>532</v>
-      </c>
-      <c r="C11" s="32">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="33">
-        <v>0.59668470406251595</v>
-      </c>
-      <c r="G11" s="33">
-        <v>0.54251543269230296</v>
-      </c>
-      <c r="H11" s="34">
-        <v>0.25319999999999998</v>
-      </c>
-      <c r="I11" s="34">
-        <v>1</v>
-      </c>
-      <c r="J11" s="35">
-        <v>0.1157</v>
-      </c>
-      <c r="K11" s="35">
-        <v>0.44490000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1">
         <v>1298</v>
       </c>
-      <c r="C12" s="32">
+      <c r="D12" s="30">
         <v>0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="34">
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="32">
         <v>0.68269999999999997</v>
       </c>
-      <c r="I12" s="34">
+      <c r="J12" s="32">
         <v>0.67910000000000004</v>
       </c>
-      <c r="J12" s="35">
+      <c r="K12" s="33">
         <v>0.72629999999999995</v>
       </c>
-      <c r="K12" s="35">
+      <c r="L12" s="33">
         <v>5.5399999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="1">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1">
         <v>537</v>
       </c>
-      <c r="C13" s="32">
+      <c r="D13" s="30">
         <v>0.13194444444444445</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="34">
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="32">
         <v>0.1595</v>
       </c>
-      <c r="I13" s="36">
+      <c r="J13" s="34">
         <v>1.9E-3</v>
       </c>
-      <c r="J13" s="35">
+      <c r="K13" s="33">
         <v>0.1303</v>
       </c>
-      <c r="K13" s="35">
+      <c r="L13" s="33">
         <v>8.3099999999999993E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="1">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1">
         <v>424</v>
       </c>
-      <c r="C14" s="32">
+      <c r="D14" s="30">
         <v>0.21527777777777779</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="31">
         <v>0.67936157811425002</v>
       </c>
-      <c r="G14" s="33">
+      <c r="H14" s="31">
         <v>0.14798711145694601</v>
       </c>
-      <c r="H14" s="36">
+      <c r="I14" s="34">
         <v>3.9300000000000002E-2</v>
       </c>
-      <c r="I14" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="37">
+      <c r="J14" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="35">
         <v>1.4500000000000001E-2</v>
       </c>
-      <c r="K14" s="35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="1">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
         <v>113</v>
       </c>
-      <c r="C15" s="32">
+      <c r="D15" s="30">
         <v>0.3125</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="31">
         <v>0.76242480909532895</v>
       </c>
-      <c r="G15" s="33">
+      <c r="H15" s="31">
         <v>0.34011786664647697</v>
       </c>
-      <c r="H15" s="34">
+      <c r="I15" s="32">
         <v>1</v>
       </c>
-      <c r="I15" s="34">
+      <c r="J15" s="32">
         <v>1</v>
       </c>
-      <c r="J15" s="35">
+      <c r="K15" s="33">
         <v>0.17199999999999999</v>
       </c>
-      <c r="K15" s="35">
+      <c r="L15" s="33">
         <v>0.77549999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="1">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
         <v>215</v>
       </c>
-      <c r="C16" s="32">
+      <c r="D16" s="30">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="34">
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="32">
         <v>0.92459999999999998</v>
       </c>
-      <c r="I16" s="34">
+      <c r="J16" s="32">
         <v>0.96179999999999999</v>
       </c>
-      <c r="J16" s="35">
+      <c r="K16" s="33">
         <v>0.45619999999999999</v>
       </c>
-      <c r="K16" s="35">
+      <c r="L16" s="33">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="1">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1">
         <v>1083</v>
       </c>
-      <c r="C17" s="32">
+      <c r="D17" s="30">
         <v>0</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="34">
+      <c r="F17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="32">
         <v>0.63600000000000001</v>
       </c>
-      <c r="I17" s="34">
+      <c r="J17" s="32">
         <v>0.57640000000000002</v>
       </c>
-      <c r="J17" s="35">
+      <c r="K17" s="33">
         <v>0.67400000000000004</v>
       </c>
-      <c r="K17" s="35">
+      <c r="L17" s="33">
         <v>0.46579999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="1">
+        <v>40</v>
+      </c>
+      <c r="C18" s="1">
         <v>1170</v>
       </c>
-      <c r="C18" s="32">
+      <c r="D18" s="30">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="34">
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="32">
         <v>0.81140000000000001</v>
       </c>
-      <c r="I18" s="34">
+      <c r="J18" s="32">
         <v>0.92310000000000003</v>
       </c>
-      <c r="J18" s="35">
+      <c r="K18" s="33">
         <v>0.80169999999999997</v>
       </c>
-      <c r="K18" s="35">
+      <c r="L18" s="33">
         <v>0.2407</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="1">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1">
         <v>329</v>
       </c>
-      <c r="C19" s="32">
+      <c r="D19" s="30">
         <v>0.1736111111111111</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="34">
+      <c r="F19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="32">
         <v>0.21590000000000001</v>
       </c>
-      <c r="I19" s="34">
+      <c r="J19" s="32">
         <v>0.47810000000000002</v>
       </c>
-      <c r="J19" s="35">
+      <c r="K19" s="33">
         <v>0.23100000000000001</v>
       </c>
-      <c r="K19" s="35">
+      <c r="L19" s="33">
         <v>0.60770000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
         <v>128</v>
       </c>
-      <c r="C20" s="32">
+      <c r="D20" s="30">
         <v>0.375</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="36">
         <v>3.0865651583756901E-2</v>
       </c>
-      <c r="G20" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="34">
+      <c r="H20" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="32">
         <v>1</v>
       </c>
-      <c r="I20" s="34">
+      <c r="J20" s="32">
         <v>1</v>
       </c>
-      <c r="J20" s="35">
+      <c r="K20" s="33">
         <v>0.2087</v>
       </c>
-      <c r="K20" s="35">
+      <c r="L20" s="33">
         <v>0.32050000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="1">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
         <v>208</v>
       </c>
-      <c r="C21" s="32">
+      <c r="D21" s="30">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="31">
         <v>0.216686556711852</v>
       </c>
-      <c r="G21" s="38">
+      <c r="H21" s="36">
         <v>2.8493285089524201E-3</v>
       </c>
-      <c r="H21" s="34">
+      <c r="I21" s="32">
         <v>0.51559999999999995</v>
       </c>
-      <c r="I21" s="34">
+      <c r="J21" s="32">
         <v>1</v>
       </c>
-      <c r="J21" s="35">
+      <c r="K21" s="33">
         <v>0.29870000000000002</v>
       </c>
-      <c r="K21" s="37">
+      <c r="L21" s="35">
         <v>3.73E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="1">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1">
         <v>955</v>
       </c>
-      <c r="C22" s="32">
+      <c r="D22" s="30">
         <v>0</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="34">
+      <c r="F22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="32">
         <v>0.72819999999999996</v>
       </c>
-      <c r="I22" s="34">
+      <c r="J22" s="32">
         <v>0.88780000000000003</v>
       </c>
-      <c r="J22" s="35">
+      <c r="K22" s="33">
         <v>0.48259999999999997</v>
       </c>
-      <c r="K22" s="35">
+      <c r="L22" s="33">
         <v>0.1905</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="1">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1">
         <v>231</v>
       </c>
-      <c r="C23" s="32">
+      <c r="D23" s="30">
         <v>0.29166666666666669</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="31">
         <v>0.41076893214743498</v>
       </c>
-      <c r="G23" s="33">
+      <c r="H23" s="31">
         <v>0.91159942440487396</v>
       </c>
-      <c r="H23" s="34">
+      <c r="I23" s="32">
         <v>1</v>
       </c>
-      <c r="I23" s="34">
+      <c r="J23" s="32">
         <v>1</v>
       </c>
-      <c r="J23" s="35">
+      <c r="K23" s="33">
         <v>0.77949999999999997</v>
       </c>
-      <c r="K23" s="35">
+      <c r="L23" s="33">
         <v>0.20680000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="1">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1">
         <v>226</v>
       </c>
-      <c r="C24" s="32">
+      <c r="D24" s="30">
         <v>0.29166666666666669</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="31">
         <v>0.41076893214743498</v>
       </c>
-      <c r="G24" s="33">
+      <c r="H24" s="31">
         <v>0.91159942440487396</v>
       </c>
-      <c r="H24" s="34">
+      <c r="I24" s="32">
         <v>1</v>
       </c>
-      <c r="I24" s="34">
+      <c r="J24" s="32">
         <v>1</v>
       </c>
-      <c r="J24" s="35">
+      <c r="K24" s="33">
         <v>0.69510000000000005</v>
       </c>
-      <c r="K24" s="35">
+      <c r="L24" s="33">
         <v>0.22450000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
         <v>5</v>
       </c>
-      <c r="C25" s="32">
+      <c r="D25" s="30">
         <v>0.96527777777777779</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="33">
+      <c r="G25" s="31">
         <v>0.85182104561004501</v>
       </c>
-      <c r="G25" s="33">
+      <c r="H25" s="31">
         <v>0.94588042864084099</v>
       </c>
-      <c r="H25" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I25" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B26" s="1">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1">
         <v>823</v>
       </c>
-      <c r="C26" s="32">
+      <c r="D26" s="30">
         <v>0</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="34">
+      <c r="F26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="32">
         <v>0.98580000000000001</v>
       </c>
-      <c r="I26" s="34">
+      <c r="J26" s="32">
         <v>0.57410000000000005</v>
       </c>
-      <c r="J26" s="35">
+      <c r="K26" s="33">
         <v>0.45679999999999998</v>
       </c>
-      <c r="K26" s="35">
+      <c r="L26" s="33">
         <v>8.1699999999999995E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="1">
+        <v>16</v>
+      </c>
+      <c r="C27" s="1">
         <v>595</v>
       </c>
-      <c r="C27" s="32">
+      <c r="D27" s="30">
         <v>0</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="34">
+      <c r="F27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="32">
         <v>0.97230000000000005</v>
       </c>
-      <c r="I27" s="34">
+      <c r="J27" s="32">
         <v>0.97240000000000004</v>
       </c>
-      <c r="J27" s="35">
+      <c r="K27" s="33">
         <v>0.35439999999999999</v>
       </c>
-      <c r="K27" s="35">
+      <c r="L27" s="33">
         <v>9.1300000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B28" s="1">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
         <v>360</v>
       </c>
-      <c r="C28" s="32">
+      <c r="D28" s="30">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="34">
+      <c r="F28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="32">
         <v>0.37259999999999999</v>
       </c>
-      <c r="I28" s="34">
+      <c r="J28" s="32">
         <v>0.87370000000000003</v>
       </c>
-      <c r="J28" s="35">
+      <c r="K28" s="33">
         <v>0.4007</v>
       </c>
-      <c r="K28" s="35">
+      <c r="L28" s="33">
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B29" s="1">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
         <v>228</v>
       </c>
-      <c r="C29" s="32">
+      <c r="D29" s="30">
         <v>0.29166666666666669</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="31">
         <v>0.41076893214743498</v>
       </c>
-      <c r="G29" s="33">
+      <c r="H29" s="31">
         <v>0.91159942440487396</v>
       </c>
-      <c r="H29" s="34">
+      <c r="I29" s="32">
         <v>1</v>
       </c>
-      <c r="I29" s="34">
+      <c r="J29" s="32">
         <v>1</v>
       </c>
-      <c r="J29" s="35">
+      <c r="K29" s="33">
         <v>0.8115</v>
       </c>
-      <c r="K29" s="35">
+      <c r="L29" s="33">
         <v>0.19320000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="1">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1">
         <v>27</v>
       </c>
-      <c r="C30" s="32">
+      <c r="D30" s="30">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="33">
+      <c r="G30" s="31">
         <v>8.0904505081459105E-2</v>
       </c>
-      <c r="G30" s="33">
+      <c r="H30" s="31">
         <v>0.114372414340387</v>
       </c>
-      <c r="H30" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I30" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="K30" s="35" t="s">
+      <c r="I30" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="33" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5621,20 +5713,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="49"/>
-    </row>
-    <row r="2" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="48"/>
+    </row>
+    <row r="2" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>138</v>
       </c>
@@ -5662,22 +5754,22 @@
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="48" t="s">
+      <c r="B3" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="46">
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
@@ -5685,22 +5777,22 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="46">
         <v>1.49E-2</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="44">
         <v>7.2599999999999998E-2</v>
       </c>
     </row>
@@ -5708,22 +5800,22 @@
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="48" t="s">
+      <c r="B5" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="44">
         <v>5.62E-2</v>
       </c>
     </row>
@@ -5731,22 +5823,22 @@
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="48" t="s">
+      <c r="B6" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="46">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="46">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
@@ -5754,22 +5846,22 @@
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="48" t="s">
+      <c r="B7" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="46" t="s">
+      <c r="F7" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="44" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5777,22 +5869,22 @@
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="48" t="s">
+      <c r="B8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="46">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="44">
         <v>6.8199999999999997E-2</v>
       </c>
     </row>
@@ -5800,22 +5892,22 @@
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="44">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="46">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="44">
         <v>0.29770000000000002</v>
       </c>
     </row>
@@ -5823,22 +5915,22 @@
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="46" t="s">
+      <c r="B10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="44">
         <v>0.60750000000000004</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="44">
         <v>0.9365</v>
       </c>
     </row>
@@ -5846,22 +5938,22 @@
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="48" t="s">
+      <c r="B11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="46">
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
@@ -5869,22 +5961,22 @@
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="48" t="s">
+      <c r="B12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="46">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="46">
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
@@ -5892,22 +5984,22 @@
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="46">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="D13" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="46" t="s">
+      <c r="D13" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="44" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5915,22 +6007,22 @@
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="44">
         <v>0.19189999999999999</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="44">
         <v>0.39779999999999999</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="44">
         <v>0.57530000000000003</v>
       </c>
     </row>
@@ -5938,22 +6030,22 @@
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="46" t="s">
+      <c r="B15" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="44">
         <v>0.65780000000000005</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="44">
         <v>0.59699999999999998</v>
       </c>
     </row>
@@ -5961,22 +6053,22 @@
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="48" t="s">
+      <c r="B16" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="46" t="s">
         <v>177</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="46">
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
@@ -5984,22 +6076,22 @@
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="48" t="s">
+      <c r="B17" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="46">
         <v>1.1299999999999999E-2</v>
       </c>
     </row>
@@ -6007,22 +6099,22 @@
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="46" t="s">
+      <c r="B18" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="44">
         <v>0.69599999999999995</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="G18" s="46">
+      <c r="G18" s="44">
         <v>0.1303</v>
       </c>
     </row>
@@ -6030,22 +6122,22 @@
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="44">
         <v>0.24629999999999999</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="44">
         <v>0.48010000000000003</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="44">
         <v>0.98380000000000001</v>
       </c>
     </row>
@@ -6053,22 +6145,22 @@
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20" s="44">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="G20" s="46">
+      <c r="G20" s="44">
         <v>7.0300000000000001E-2</v>
       </c>
     </row>
@@ -6076,22 +6168,22 @@
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="46" t="s">
+      <c r="B21" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="44">
         <v>0.42270000000000002</v>
       </c>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="44">
         <v>0.72060000000000002</v>
       </c>
     </row>
@@ -6099,22 +6191,22 @@
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22" s="44">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="46" t="s">
         <v>216</v>
       </c>
     </row>
@@ -6122,22 +6214,22 @@
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="46">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="G23" s="48" t="s">
+      <c r="G23" s="46" t="s">
         <v>216</v>
       </c>
     </row>
@@ -6145,22 +6237,22 @@
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C24" s="44">
         <v>0.19189999999999999</v>
       </c>
-      <c r="D24" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="46" t="s">
+      <c r="D24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="44" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6168,22 +6260,22 @@
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="46" t="s">
+      <c r="B25" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="E25" s="46">
+      <c r="E25" s="44">
         <v>0.54059999999999997</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="G25" s="46">
+      <c r="G25" s="44">
         <v>0.51200000000000001</v>
       </c>
     </row>
@@ -6191,22 +6283,22 @@
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="46" t="s">
+      <c r="B26" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="44">
         <v>9.8599999999999993E-2</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="48">
+      <c r="G26" s="46">
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
@@ -6214,22 +6306,22 @@
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="48" t="s">
+      <c r="B27" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="48">
+      <c r="G27" s="46">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
@@ -6237,22 +6329,22 @@
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="C28" s="46">
+      <c r="C28" s="44">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="G28" s="48">
+      <c r="G28" s="46">
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
@@ -6260,22 +6352,22 @@
       <c r="A29" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="44">
         <v>0.24629999999999999</v>
       </c>
-      <c r="D29" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="46" t="s">
+      <c r="D29" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="44" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6368,28 +6460,28 @@
       <c r="C3" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="39">
         <v>1836</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="41">
         <v>0.104166667</v>
       </c>
-      <c r="F3" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="44">
+      <c r="F3" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="42">
         <v>0.97719999999999996</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="42">
         <v>1</v>
       </c>
-      <c r="J3" s="45">
+      <c r="J3" s="43">
         <v>2.5100000000000001E-2</v>
       </c>
-      <c r="K3" s="44">
+      <c r="K3" s="42">
         <v>0.1231</v>
       </c>
     </row>
@@ -6403,28 +6495,28 @@
       <c r="C4" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="39">
         <v>369</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="41">
         <v>0.51388888899999996</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="42">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="I4" s="45">
+      <c r="I4" s="43">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="J4" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="44" t="s">
+      <c r="J4" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="42" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6438,28 +6530,28 @@
       <c r="C5" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="39">
         <v>1816</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="41">
         <v>6.25E-2</v>
       </c>
-      <c r="F5" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="44">
+      <c r="F5" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="42">
         <v>0.7429</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="42">
         <v>1</v>
       </c>
-      <c r="J5" s="45">
+      <c r="J5" s="43">
         <v>0</v>
       </c>
-      <c r="K5" s="44">
+      <c r="K5" s="42">
         <v>0.69210000000000005</v>
       </c>
     </row>
@@ -6485,16 +6577,16 @@
       <c r="G6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="37">
         <v>0.1779</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="37">
         <v>0.1125</v>
       </c>
-      <c r="J6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="39" t="s">
+      <c r="J6" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="37" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6520,16 +6612,16 @@
       <c r="G7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="37">
         <v>0.32429999999999998</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="37">
         <v>0.38419999999999999</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="37">
         <v>0.87280000000000002</v>
       </c>
     </row>
@@ -6555,16 +6647,16 @@
       <c r="G8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="37">
         <v>1</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="37">
         <v>0.77010000000000001</v>
       </c>
-      <c r="J8" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="39" t="s">
+      <c r="J8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="37" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6590,16 +6682,16 @@
       <c r="G9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="37">
         <v>0.71319999999999995</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="37">
         <v>0.88249999999999995</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="37">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="37">
         <v>0.63249999999999995</v>
       </c>
     </row>
@@ -6625,22 +6717,22 @@
       <c r="G10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="37">
         <v>0.84489999999999998</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="37">
         <v>0.83720000000000006</v>
       </c>
-      <c r="J10" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="39" t="s">
+      <c r="J10" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="J12" s="41"/>
-      <c r="K12" s="40"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>